<commit_message>
fix: csv files can now be added to the page
- made barriers non-existent when highlighting
- changes to templates
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Scholar Application.xlsx
+++ b/frontend/src/components/components/Scholar Application.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>SCHOLARVISION APPLICANT INFORMATION</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Email *</t>
   </si>
   <si>
-    <t>Street Name, House No. *</t>
-  </si>
-  <si>
     <t>Subdivision *</t>
   </si>
   <si>
@@ -214,6 +211,12 @@
   </si>
   <si>
     <t>Postal Code *</t>
+  </si>
+  <si>
+    <t>Street Name &amp; House No. *</t>
+  </si>
+  <si>
+    <t>Student Number *</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -234,40 +237,47 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color rgb="FFFFFFFF"/>
       <name val="Corbel"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Corbel"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF52565E"/>
       <name val="Corbel"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFEF2"/>
       <name val="Corbel"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -280,6 +290,17 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Corbel"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -756,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -806,39 +827,34 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -847,9 +863,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -860,10 +880,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1088,11 +1116,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="B70:F70"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1116,613 +1144,615 @@
     </row>
     <row r="2" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="21"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="21"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="21"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="21"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="19"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="21"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33"/>
+      <c r="B12" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="24"/>
+      <c r="B13" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="51"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="21"/>
+      <c r="B14" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="22"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="44"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="21"/>
+      <c r="B15" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="30"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="19"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="43" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
+      <c r="B17" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="44"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
+      <c r="B18" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="44"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
+      <c r="B19" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="19"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="44"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
+      <c r="B20" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="30"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="44"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
+      <c r="B21" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
-      <c r="B22" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="21"/>
+      <c r="B22" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="24"/>
+      <c r="B23" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
-      <c r="B24" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="24"/>
+      <c r="B24" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21"/>
+      <c r="B25" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
+      <c r="B26" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="21"/>
+      <c r="B27" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="24"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
+      <c r="B28" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
+      <c r="B29" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="24"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="19"/>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
+      <c r="B30" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
-      <c r="B31" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="18"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
+      <c r="B31" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="21"/>
+      <c r="B32" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
-      <c r="B33" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="21"/>
+      <c r="B33" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="19"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="24"/>
+      <c r="B34" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="24"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="21"/>
+      <c r="B35" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="22"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
-      <c r="B36" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="21"/>
+      <c r="B36" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="24"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="21"/>
+      <c r="B37" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="24"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="21"/>
+      <c r="B38" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38" s="24"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
-      <c r="B39" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="21"/>
+      <c r="B39" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
-      <c r="B40" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="18"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="21"/>
+      <c r="B40" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="24"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="18"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="21"/>
+      <c r="B41" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="24"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
-      <c r="B42" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="21"/>
+      <c r="B42" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="24"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
-      <c r="B43" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="18"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="21"/>
+      <c r="B43" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="24"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="24"/>
+      <c r="B44" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="24"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
-      <c r="B45" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="18"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="21"/>
+      <c r="B45" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="22"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
-      <c r="B46" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="21"/>
+      <c r="B46" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="24"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="19"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="21"/>
+      <c r="B47" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="24"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="19"/>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
-      <c r="B48" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="18"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="21"/>
+      <c r="B48" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="24"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="19"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
-      <c r="B49" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="21"/>
+      <c r="B49" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="24"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="19"/>
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="21"/>
+      <c r="B50" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="24"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="19"/>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
-      <c r="B51" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="18"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="21"/>
+      <c r="B51" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="24"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="19"/>
       <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
-      <c r="B52" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="21"/>
+      <c r="B52" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="24"/>
+      <c r="D52" s="17"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="19"/>
       <c r="G52" s="4"/>
     </row>
     <row r="53" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
-      <c r="B53" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="21"/>
+      <c r="B53" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="24"/>
+      <c r="D53" s="17"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="19"/>
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
-      <c r="B54" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
-      <c r="F54" s="24"/>
+      <c r="B54" s="42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="43"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="19"/>
       <c r="G54" s="4"/>
     </row>
     <row r="55" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
-      <c r="B55" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>42</v>
-      </c>
+      <c r="B55" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="22"/>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="10"/>
+      <c r="B56" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
@@ -1763,48 +1793,48 @@
     </row>
     <row r="61" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="12"/>
-      <c r="D61" s="12"/>
-      <c r="E61" s="12"/>
-      <c r="F61" s="13"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="10"/>
       <c r="G61" s="4"/>
     </row>
     <row r="62" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
-      <c r="B62" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="28"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="13"/>
       <c r="G62" s="4"/>
     </row>
     <row r="63" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
-      <c r="B63" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E63" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="F63" s="36"/>
+      <c r="B63" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="39"/>
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="9"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="36"/>
+      <c r="B64" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E64" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F64" s="33"/>
       <c r="G64" s="4"/>
     </row>
     <row r="65" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
@@ -1812,8 +1842,8 @@
       <c r="B65" s="8"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="36"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="33"/>
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
@@ -1821,8 +1851,8 @@
       <c r="B66" s="8"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
-      <c r="E66" s="40"/>
-      <c r="F66" s="36"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="33"/>
       <c r="G66" s="4"/>
     </row>
     <row r="67" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
@@ -1830,78 +1860,153 @@
       <c r="B67" s="8"/>
       <c r="C67" s="9"/>
       <c r="D67" s="9"/>
-      <c r="E67" s="40"/>
-      <c r="F67" s="36"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="49"/>
       <c r="G67" s="4"/>
     </row>
     <row r="68" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
-      <c r="B68" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="28"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="33"/>
       <c r="G68" s="4"/>
     </row>
     <row r="69" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
-      <c r="B69" s="34" t="s">
+      <c r="B69" s="8"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="38"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="38"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="4"/>
-    </row>
-    <row r="70" spans="1:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="37"/>
-      <c r="C70" s="32"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="4"/>
-    </row>
-    <row r="71" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="1"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="4"/>
+    </row>
+    <row r="72" spans="1:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="34"/>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="4"/>
+    </row>
+    <row r="73" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="106">
+  <mergeCells count="109">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B71:F71"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B63:F63"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E65:F65"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:F52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D42:F42"/>
     <mergeCell ref="D47:F47"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D48:F48"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:F42"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="D43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="D46:F46"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="B37:C37"/>
@@ -1910,85 +2015,31 @@
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="D39:F39"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B69:F69"/>
-    <mergeCell ref="B70:F70"/>
-    <mergeCell ref="D53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:F52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="B68:F68"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D40:F40"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D9">
       <formula1>"M,F"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a number!" sqref="D14 D33 D43 D53 C56:C61">
-      <formula1>REGEXMATCH(TO_TEXT(C14), "^[0-9]*$")</formula1>
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a number!" sqref="D15 D34 D44 D54 C57:C62">
+      <formula1>REGEXMATCH(TO_TEXT(C15), "^[0-9]*$")</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a date!" sqref="D8">
       <formula1>OR(NOT(ISERROR(DATEVALUE(D8))), AND(ISNUMBER(D8), LEFT(CELL("format", D8))="D"))</formula1>

</xml_diff>

<commit_message>
fix: updated Excel file for application
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Scholar Application.xlsx
+++ b/frontend/src/components/components/Scholar Application.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\OneDrive - up.edu.ph\Documents\CMSC\2SP\frontend\src\components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\OneDrive - up.edu.ph\Documents\GitHub\ScholarVision\frontend\src\components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -345,7 +345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -776,11 +776,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -901,6 +914,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,8 +1141,8 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1400,20 +1419,20 @@
     </row>
     <row r="25" spans="1:7" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="19"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="53"/>
+      <c r="F25" s="52"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="41"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="19"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="52"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.3">
@@ -1988,10 +2007,10 @@
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D25:F25"/>
     <mergeCell ref="D26:F26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:F25"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="D4:F4"/>
@@ -2072,15 +2091,15 @@
     <mergeCell ref="B37:C37"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D9">
-      <formula1>"M,F"</formula1>
-    </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a number!" sqref="D15 D37 D47 D57 C60:C65">
       <formula1>REGEXMATCH(TO_TEXT(C15), "^[0-9]*$")</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Must be a date!" sqref="D8">
       <formula1>OR(NOT(ISERROR(DATEVALUE(D8))), AND(ISNUMBER(D8), LEFT(CELL("format", D8))="D"))</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D9:F9">
+      <formula1>"male,female"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>